<commit_message>
Update NonToxicScore with DistilBERT Upsampling 512 tokens
</commit_message>
<xml_diff>
--- a/models/model_weights.xlsx
+++ b/models/model_weights.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b0bc52a19a20cdd0/w266/style_transfer_w266/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{761940F0-E177-4EF4-9B06-E26DE5C34216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDAE74CD-694F-4822-B4A6-B1ACBF1A2464}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{761940F0-E177-4EF4-9B06-E26DE5C34216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEC0101C-0E0D-4995-90FD-B08028EF2E5A}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0DAB5342-1498-4B72-B08C-503E886F2C71}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Model</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Others</t>
   </si>
   <si>
-    <t>scheduler Tmax = epochs = 4</t>
-  </si>
-  <si>
     <t>last transformer layer</t>
   </si>
   <si>
@@ -129,6 +126,24 @@
   </si>
   <si>
     <t>Oversampling</t>
+  </si>
+  <si>
+    <t>1 hidden layer</t>
+  </si>
+  <si>
+    <t>1 hidden layer. scheduler Tmax = epochs = 4</t>
+  </si>
+  <si>
+    <t>DistilBertToxicClassification512tok.pth</t>
+  </si>
+  <si>
+    <t>2 hidden layers, , GELU(), 2 epochs. 512 tokens</t>
+  </si>
+  <si>
+    <t>DistilBertToxicClassification6.pth</t>
+  </si>
+  <si>
+    <t>DistilBertToxicClassification7.pth</t>
   </si>
 </sst>
 </file>
@@ -186,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -197,6 +212,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,6 +234,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -512,11 +537,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78377F24-0200-48F8-A77D-C90262A2D0EF}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,10 +550,10 @@
     <col min="2" max="2" width="17.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="7" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -537,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -551,7 +576,7 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -561,10 +586,10 @@
         <v>11</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>17</v>
@@ -589,7 +614,7 @@
       <c r="F2">
         <v>16</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="7">
         <v>384</v>
       </c>
       <c r="H2">
@@ -621,7 +646,7 @@
       <c r="F3">
         <v>16</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="7">
         <v>768</v>
       </c>
       <c r="H3">
@@ -631,11 +656,14 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" t="s">
         <v>10</v>
       </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -656,7 +684,7 @@
       <c r="F4">
         <v>16</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <v>768</v>
       </c>
       <c r="H4">
@@ -666,11 +694,14 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" t="s">
         <v>8</v>
       </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -691,7 +722,7 @@
       <c r="F5">
         <v>16</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>768</v>
       </c>
       <c r="H5">
@@ -701,11 +732,14 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5" t="s">
         <v>14</v>
       </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -726,8 +760,8 @@
       <c r="F6">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
-        <v>24</v>
+      <c r="G6" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="H6">
         <v>0.1</v>
@@ -736,13 +770,13 @@
         <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -764,23 +798,23 @@
       <c r="F7">
         <v>16</v>
       </c>
-      <c r="G7" t="s">
-        <v>24</v>
+      <c r="G7" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="H7">
         <v>0.1</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -802,8 +836,8 @@
       <c r="F8">
         <v>16</v>
       </c>
-      <c r="G8" t="s">
-        <v>24</v>
+      <c r="G8" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="H8">
         <v>0.1</v>
@@ -812,13 +846,13 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -828,6 +862,7 @@
       <c r="B9" s="2">
         <v>1</v>
       </c>
+      <c r="C9" s="5"/>
       <c r="D9">
         <v>64</v>
       </c>
@@ -837,8 +872,8 @@
       <c r="F9">
         <v>16</v>
       </c>
-      <c r="G9" t="s">
-        <v>24</v>
+      <c r="G9" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="H9">
         <v>0.1</v>
@@ -847,21 +882,21 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>31</v>
       </c>
       <c r="L9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B10" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="C10">
-        <v>0.90769999999999995</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>64</v>
@@ -872,8 +907,8 @@
       <c r="F10">
         <v>16</v>
       </c>
-      <c r="G10">
-        <v>768</v>
+      <c r="G10" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="H10">
         <v>0.1</v>
@@ -885,30 +920,30 @@
         <v>28</v>
       </c>
       <c r="K10" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="L10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="C11">
-        <v>0.89339999999999997</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>64</v>
       </c>
       <c r="E11" s="1">
-        <v>1E-4</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="F11">
         <v>16</v>
       </c>
-      <c r="G11">
-        <v>768</v>
+      <c r="G11" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="H11">
         <v>0.1</v>
@@ -920,10 +955,10 @@
         <v>28</v>
       </c>
       <c r="K11" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="L11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -931,21 +966,21 @@
         <v>13</v>
       </c>
       <c r="B12" s="2">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C12">
-        <v>0.89219999999999999</v>
+        <v>0.90769999999999995</v>
       </c>
       <c r="D12">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E12" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="F12">
         <v>16</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="7">
         <v>768</v>
       </c>
       <c r="H12">
@@ -955,14 +990,93 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="L12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C13">
+        <v>0.89339999999999997</v>
+      </c>
+      <c r="D13">
+        <v>64</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F13">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7">
+        <v>768</v>
+      </c>
+      <c r="H13">
+        <v>0.1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C14">
+        <v>0.89219999999999999</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F14">
+        <v>16</v>
+      </c>
+      <c r="G14" s="7">
+        <v>768</v>
+      </c>
+      <c r="H14">
+        <v>0.1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L12" xr:uid="{78377F24-0200-48F8-A77D-C90262A2D0EF}"/>
+  <autoFilter ref="A1:L14" xr:uid="{78377F24-0200-48F8-A77D-C90262A2D0EF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>